<commit_message>
Fixed nowcast-error and implemented  refinements for nowcasting in, out-of sample
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance.xlsx
+++ b/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb59f80414e38fcc/Documentos/RA/CIUP/GDP Revisions/GitHub/peru_gdp_revisions/gdp_revisions_analysis_jefas/input/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Cruz\OneDrive\Documentos\RA\CIUP\GDP Revisions\GitHub\peru_gdp_revisions\gdp_revisions_analysis_jefas\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_B35981270C0FB91E2035D31957411812710406EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{538805C4-94A0-445B-86BD-056E6639EBFD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F535879A-9666-4683-A41B-52E12B9FDC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,38 +20,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Horizon</t>
+  </si>
+  <si>
+    <t>RMSE (Bench=100)</t>
+  </si>
   <si>
     <t>DM stat</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>RMSE
-(Bench=100)</t>
-  </si>
-  <si>
-    <t>Encom
-β t-stat</t>
-  </si>
-  <si>
-    <t>SS</t>
+    <t>Encompassing t-stat β</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,60 +67,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,10 +91,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,204 +410,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>85.8211669921875</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-2.0147576332092285</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.213951587677002</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8">
-        <v>58.993988037109375</v>
-      </c>
-      <c r="C3" s="8">
-        <v>-3.0478553771972656</v>
-      </c>
-      <c r="D3" s="8">
-        <v>32.442737579345703</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>86.935012817382813</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-1.8162939548492432</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.1529755592346191</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>60.809337615966797</v>
-      </c>
-      <c r="C4" s="3">
-        <v>-2.6771316528320313</v>
-      </c>
-      <c r="D4" s="3">
-        <v>24.950651168823242</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>85.535331726074219</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-1.3983992338180542</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.5278384685516357</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>60.849075317382813</v>
-      </c>
-      <c r="C5" s="3">
-        <v>-2.9272449016571045</v>
-      </c>
-      <c r="D5" s="3">
-        <v>14.666155815124512</v>
-      </c>
-      <c r="E5" s="4"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>94.562545776367188</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-1.0848034620285034</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.7606265544891357</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>50.121318817138672</v>
-      </c>
-      <c r="C6" s="3">
-        <v>-3.0377659797668457</v>
-      </c>
-      <c r="D6" s="3">
-        <v>30.750665664672852</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>97.852302551269531</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-0.54339373111724854</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.9575998783111572</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>42.675712585449219</v>
-      </c>
-      <c r="C7" s="3">
-        <v>-3.2964847087860107</v>
-      </c>
-      <c r="D7" s="3">
-        <v>44.789279937744141</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>94.610992431640625</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-0.80235564708709717</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.6346943378448486</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>46.551906585693359</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-3.0134758949279785</v>
-      </c>
-      <c r="D8" s="3">
-        <v>22.311849594116211</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>97.575553894042969</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-0.77277088165283203</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.3231902122497559</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3">
-        <v>33.451381683349609</v>
-      </c>
-      <c r="C9" s="3">
-        <v>-3.0740752220153809</v>
-      </c>
-      <c r="D9" s="3">
-        <v>28.689947128295898</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>99.357131958007813</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-0.45807769894599915</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.5395486354827881</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3">
-        <v>15.478214263916016</v>
-      </c>
-      <c r="C10" s="3">
-        <v>-3.1853504180908203</v>
-      </c>
-      <c r="D10" s="3">
-        <v>140.14883422851563</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>99.1380615234375</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1.1757581233978271</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.1389737129211426</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3">
-        <v>9.7826204299926758</v>
-      </c>
-      <c r="C11" s="3">
-        <v>-2.7026569843292236</v>
-      </c>
-      <c r="D11" s="3">
-        <v>171.966064453125</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>99.222213745117188</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-1.5714582204818726</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5.0303716659545898</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3">
-        <v>18.186698913574219</v>
-      </c>
-      <c r="C12" s="3">
-        <v>-2.9087696075439453</v>
-      </c>
-      <c r="D12" s="3">
-        <v>122.86335754394531</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="10">
-        <v>12.608890533447266</v>
-      </c>
-      <c r="C13" s="10">
-        <v>-2.2478878498077393</v>
-      </c>
-      <c r="D13" s="10">
-        <v>143.07743835449219</v>
-      </c>
-    </row>
-    <row r="21" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J21" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B12" s="2">
+        <v>100.01242065429688</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1.6048025339841843E-2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.89620393514633179</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Interchanged section for WES creation and Regressions
</commit_message>
<xml_diff>
--- a/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance.xlsx
+++ b/gdp_revisions_analysis_jefas/input/data/Nowcasting_Performance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Cruz\OneDrive\Documentos\RA\CIUP\GDP Revisions\GitHub\peru_gdp_revisions\gdp_revisions_analysis_jefas\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F535879A-9666-4683-A41B-52E12B9FDC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F9E453-6BA9-4002-BC29-3B11F8776CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,26 +22,33 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Horizon</t>
-  </si>
-  <si>
-    <t>RMSE (Bench=100)</t>
-  </si>
-  <si>
     <t>DM stat</t>
   </si>
   <si>
-    <t>Encompassing t-stat β</t>
+    <t>RMSE
+(Bench=100)</t>
+  </si>
+  <si>
+    <t>Encom
+β t-stat</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -67,15 +74,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,197 +455,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E2" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="1">
+        <v>85.8046875</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-2.3395786285400391</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.1634807586669922</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C4" s="1">
+        <v>86.504852294921875</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-2.2288544178009033</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.1357460021972656</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>85.8211669921875</v>
-      </c>
-      <c r="C2" s="2">
-        <v>-2.0147576332092285</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2.213951587677002</v>
-      </c>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>86.935012817382813</v>
-      </c>
-      <c r="C3" s="2">
-        <v>-1.8162939548492432</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.1529755592346191</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>85.535331726074219</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-1.3983992338180542</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3.5278384685516357</v>
-      </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="C5" s="1">
+        <v>84.671028137207031</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-1.5281746387481689</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.1056637763977051</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>94.562545776367188</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-1.0848034620285034</v>
-      </c>
-      <c r="D5" s="2">
-        <v>2.7606265544891357</v>
-      </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="C6" s="1">
+        <v>93.787605285644531</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-1.8327193260192871</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.1704645156860352</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>97.852302551269531</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-0.54339373111724854</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1.9575998783111572</v>
-      </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="C7" s="1">
+        <v>96.509185791015625</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-1.4499260187149048</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.9902466535568237</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>94.610992431640625</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-0.80235564708709717</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2.6346943378448486</v>
-      </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="C8" s="1">
+        <v>93.883811950683594</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-1.0173096656799316</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.3546054363250732</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>97.575553894042969</v>
-      </c>
-      <c r="C8" s="2">
-        <v>-0.77277088165283203</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2.3231902122497559</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="C9" s="1">
+        <v>97.242012023925781</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-1.1992597579956055</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.4979555606842041</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>99.357131958007813</v>
-      </c>
-      <c r="C9" s="2">
-        <v>-0.45807769894599915</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.5395486354827881</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+      <c r="C10" s="1">
+        <v>99.411849975585938</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-0.39264366030693054</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.93626856803894043</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>99.1380615234375</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-1.1757581233978271</v>
-      </c>
-      <c r="D10" s="2">
-        <v>2.1389737129211426</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+      <c r="C11" s="1">
+        <v>99.504592895507813</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-0.89987170696258545</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.6724241971969604</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>99.222213745117188</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-1.5714582204818726</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5.0303716659545898</v>
-      </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="C12" s="1">
+        <v>99.725357055664063</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1.1257961988449097</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.3600287437438965</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>100.01242065429688</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1.6048025339841843E-2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.89620393514633179</v>
-      </c>
-      <c r="E12" s="3"/>
+      <c r="C13" s="5">
+        <v>99.830368041992188</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-0.55875509977340698</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1.2645409107208252</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>